<commit_message>
plots ejercicio 6, falta el ejercicio 6 corregido
</commit_message>
<xml_diff>
--- a/plots/plots-ej6/resumen_lambda.xlsx
+++ b/plots/plots-ej6/resumen_lambda.xlsx
@@ -505,37 +505,37 @@
         <v>0.02</v>
       </c>
       <c r="B2" t="n">
-        <v>0.09765444444444445</v>
+        <v>0.09757222222222223</v>
       </c>
       <c r="C2" t="n">
-        <v>0.0003129040568692145</v>
+        <v>0.0003127865507069558</v>
       </c>
       <c r="D2" t="n">
         <v>900000</v>
       </c>
       <c r="E2" t="n">
-        <v>0.09272311754395048</v>
+        <v>0.09256073464898067</v>
       </c>
       <c r="F2" t="n">
-        <v>0.0002788792110986285</v>
+        <v>0.000278872105027218</v>
       </c>
       <c r="G2" t="n">
-        <v>1081672</v>
+        <v>1080026</v>
       </c>
       <c r="H2" t="n">
-        <v>0.04438961163827852</v>
+        <v>0.04452022451311358</v>
       </c>
       <c r="I2" t="n">
-        <v>0.0001980310590181541</v>
+        <v>0.0001984596938272205</v>
       </c>
       <c r="J2" t="n">
-        <v>1081672</v>
+        <v>1080026</v>
       </c>
       <c r="K2" t="n">
-        <v>0</v>
+        <v>0.01128633574592749</v>
       </c>
       <c r="L2" t="n">
-        <v>0</v>
+        <v>8.266279737757257e-05</v>
       </c>
       <c r="M2" t="inlineStr">
         <is>
@@ -548,37 +548,37 @@
         <v>0.1</v>
       </c>
       <c r="B3" t="n">
-        <v>0.8381044444444444</v>
+        <v>0.8376977777777778</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0003882802319157784</v>
+        <v>0.0003886732573539983</v>
       </c>
       <c r="D3" t="n">
         <v>900000</v>
       </c>
       <c r="E3" t="n">
-        <v>0.3891462304976275</v>
+        <v>0.3889321431328914</v>
       </c>
       <c r="F3" t="n">
-        <v>0.00020975898908415</v>
+        <v>0.0002097728379262024</v>
       </c>
       <c r="G3" t="n">
-        <v>5402676</v>
+        <v>5400883</v>
       </c>
       <c r="H3" t="n">
-        <v>0.09628006565635251</v>
+        <v>0.09611243198565864</v>
       </c>
       <c r="I3" t="n">
-        <v>0.0001269055624202617</v>
+        <v>0.000126827842691839</v>
       </c>
       <c r="J3" t="n">
-        <v>5402676</v>
+        <v>5400883</v>
       </c>
       <c r="K3" t="n">
-        <v>0</v>
+        <v>0.05807639207557461</v>
       </c>
       <c r="L3" t="n">
-        <v>0</v>
+        <v>8.835601281472285e-05</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>
@@ -591,37 +591,37 @@
         <v>0.2</v>
       </c>
       <c r="B4" t="n">
-        <v>0.9947211111111111</v>
+        <v>0.9947233333333333</v>
       </c>
       <c r="C4" t="n">
-        <v>7.638369678426665e-05</v>
+        <v>7.636770300152048e-05</v>
       </c>
       <c r="D4" t="n">
         <v>900000</v>
       </c>
       <c r="E4" t="n">
-        <v>0.6259749850045049</v>
+        <v>0.6260722349197325</v>
       </c>
       <c r="F4" t="n">
-        <v>0.0001472489699650987</v>
+        <v>0.0001472261831356737</v>
       </c>
       <c r="G4" t="n">
-        <v>10798243</v>
+        <v>10800455</v>
       </c>
       <c r="H4" t="n">
-        <v>0.1858750539323851</v>
+        <v>0.1859705910538028</v>
       </c>
       <c r="I4" t="n">
-        <v>0.0001183803273992593</v>
+        <v>0.0001183916729308955</v>
       </c>
       <c r="J4" t="n">
-        <v>10798243</v>
+        <v>10800455</v>
       </c>
       <c r="K4" t="n">
-        <v>0</v>
+        <v>0.111800217070816</v>
       </c>
       <c r="L4" t="n">
-        <v>0</v>
+        <v>9.214605088138318e-05</v>
       </c>
       <c r="M4" t="inlineStr">
         <is>
@@ -643,28 +643,28 @@
         <v>900000</v>
       </c>
       <c r="E5" t="n">
-        <v>0.9039872201707653</v>
+        <v>0.9040107740053344</v>
       </c>
       <c r="F5" t="n">
-        <v>5.670795259149788e-05</v>
+        <v>5.669147628739128e-05</v>
       </c>
       <c r="G5" t="n">
-        <v>26990032</v>
+        <v>26999801</v>
       </c>
       <c r="H5" t="n">
-        <v>0.4552959774186263</v>
+        <v>0.4556105802409433</v>
       </c>
       <c r="I5" t="n">
-        <v>9.58573675519783e-05</v>
+        <v>9.584544029742404e-05</v>
       </c>
       <c r="J5" t="n">
-        <v>26990032</v>
+        <v>26999801</v>
       </c>
       <c r="K5" t="n">
-        <v>0</v>
+        <v>0.2685176288677825</v>
       </c>
       <c r="L5" t="n">
-        <v>0</v>
+        <v>9.637905349392552e-05</v>
       </c>
       <c r="M5" t="inlineStr">
         <is>
@@ -686,28 +686,28 @@
         <v>900000</v>
       </c>
       <c r="E6" t="n">
-        <v>0.9683787037037037</v>
+        <v>0.9683777037037037</v>
       </c>
       <c r="F6" t="n">
-        <v>2.381307994018714e-05</v>
+        <v>2.381344417715802e-05</v>
       </c>
       <c r="G6" t="n">
         <v>54000000</v>
       </c>
       <c r="H6" t="n">
-        <v>0.6076706296296296</v>
+        <v>0.6077662777777778</v>
       </c>
       <c r="I6" t="n">
-        <v>6.644505325554775e-05</v>
+        <v>6.64421816839611e-05</v>
       </c>
       <c r="J6" t="n">
         <v>54000000</v>
       </c>
       <c r="K6" t="n">
-        <v>0</v>
+        <v>0.5904021657362619</v>
       </c>
       <c r="L6" t="n">
-        <v>0</v>
+        <v>2.137981728407834e-05</v>
       </c>
       <c r="M6" t="inlineStr">
         <is>

</xml_diff>